<commit_message>
Temples webpage completed all pages.
</commit_message>
<xml_diff>
--- a/project/data/temples-web.xlsx
+++ b/project/data/temples-web.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdixon\Dropbox\My Documents\Personal\School\wdd231\project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30735C3A-5E22-4E97-A0EF-A2D9B1B944A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD5F288-E349-43D1-8499-F16DB4257061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31290" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temples" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2919" uniqueCount="1905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2932" uniqueCount="1917">
   <si>
     <t>Temple</t>
   </si>
@@ -5756,6 +5756,42 @@
   </si>
   <si>
     <t>images/temples/grand-junction-colorado-temple-57828-main.webp</t>
+  </si>
+  <si>
+    <t>1/31/1871</t>
+  </si>
+  <si>
+    <t>7/28/1847</t>
+  </si>
+  <si>
+    <t>4/6/1893</t>
+  </si>
+  <si>
+    <t>10/6/1876</t>
+  </si>
+  <si>
+    <t>6/25/1875</t>
+  </si>
+  <si>
+    <t>11/9/1871</t>
+  </si>
+  <si>
+    <t>5/18/1877</t>
+  </si>
+  <si>
+    <t>4/25/1877</t>
+  </si>
+  <si>
+    <t>2/14/1853</t>
+  </si>
+  <si>
+    <t>4/6/1877</t>
+  </si>
+  <si>
+    <t>5/17/1884</t>
+  </si>
+  <si>
+    <t>5/21/1888</t>
   </si>
 </sst>
 </file>
@@ -5777,16 +5813,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -5808,6 +5847,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6206,10 +6246,10 @@
   <dimension ref="A1:AE612"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P213" sqref="P213"/>
+      <selection pane="bottomRight" activeCell="F208" sqref="F208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -6290,14 +6330,14 @@
       <c r="B2" s="7" t="s">
         <v>1221</v>
       </c>
-      <c r="C2" s="9">
-        <v>25964</v>
-      </c>
-      <c r="D2" s="9">
-        <v>26246</v>
-      </c>
-      <c r="E2" s="9">
-        <v>28221</v>
+      <c r="C2" s="9" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>1910</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>1914</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>13</v>
@@ -6344,14 +6384,14 @@
       <c r="B3" s="7" t="s">
         <v>985</v>
       </c>
-      <c r="C3" s="9">
-        <v>28039</v>
-      </c>
-      <c r="D3" s="9">
-        <v>28263</v>
-      </c>
-      <c r="E3" s="9">
-        <v>30819</v>
+      <c r="C3" s="9" t="s">
+        <v>1908</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>1911</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>1915</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>19</v>
@@ -6394,14 +6434,14 @@
       <c r="B4" s="7" t="s">
         <v>1011</v>
       </c>
-      <c r="C4" s="9">
-        <v>27570</v>
-      </c>
-      <c r="D4" s="9">
-        <v>28240</v>
-      </c>
-      <c r="E4" s="9">
-        <v>32284</v>
+      <c r="C4" s="9" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1912</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>1916</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>23</v>
@@ -6448,14 +6488,14 @@
       <c r="B5" s="13" t="s">
         <v>1175</v>
       </c>
-      <c r="C5" s="9">
-        <v>17376</v>
-      </c>
-      <c r="D5" s="9">
-        <v>19404</v>
-      </c>
-      <c r="E5" s="9">
-        <v>34065</v>
+      <c r="C5" s="9" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>1913</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>1907</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>27</v>
@@ -16690,7 +16730,9 @@
       <c r="E207" s="23">
         <v>45816</v>
       </c>
-      <c r="F207" s="7"/>
+      <c r="F207" s="7" t="s">
+        <v>465</v>
+      </c>
       <c r="G207" s="8">
         <v>206</v>
       </c>

</xml_diff>